<commit_message>
Include project planing and mgt tasks
Tasks for the project planing and management included
</commit_message>
<xml_diff>
--- a/Project_Management.xlsx
+++ b/Project_Management.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7630" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasks" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks Tech" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks Mgt" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="182">
   <si>
     <t>Task</t>
   </si>
@@ -347,6 +348,231 @@
   </si>
   <si>
     <t>Web Design</t>
+  </si>
+  <si>
+    <t>Project Planning</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>State of the art</t>
+  </si>
+  <si>
+    <t>Define project management tool</t>
+  </si>
+  <si>
+    <t>Set project deadlines</t>
+  </si>
+  <si>
+    <t>Describe project tasks</t>
+  </si>
+  <si>
+    <t>Identify options to make money transfer</t>
+  </si>
+  <si>
+    <t>Agree on available budget for phase 1</t>
+  </si>
+  <si>
+    <t>Decide on money transfer method</t>
+  </si>
+  <si>
+    <t>Transfer initial part of budget</t>
+  </si>
+  <si>
+    <t>Transfer second part of budget</t>
+  </si>
+  <si>
+    <t>Integrate project timeline in project management tool</t>
+  </si>
+  <si>
+    <t>Create project timeline in Excel</t>
+  </si>
+  <si>
+    <t>Create project timeline in project management tool</t>
+  </si>
+  <si>
+    <t>Create accounting list</t>
+  </si>
+  <si>
+    <t>Identify main competitors</t>
+  </si>
+  <si>
+    <t>Create company profile of main competitors</t>
+  </si>
+  <si>
+    <t>Investigate characteristics of analog multiplexers</t>
+  </si>
+  <si>
+    <t>Research on MCUs or platforms available for prototyping (e.g., Arduino, Raspberry Pi)</t>
+  </si>
+  <si>
+    <t>Market Research</t>
+  </si>
+  <si>
+    <t>Business Plan</t>
+  </si>
+  <si>
+    <t>Evaluate market size and expected growth for electronic medical devices</t>
+  </si>
+  <si>
+    <t>Evaluate market size and expected growth for eHealth</t>
+  </si>
+  <si>
+    <t>Evaluate market size and expected growth for development microcontroller platforms</t>
+  </si>
+  <si>
+    <t>Create list of components necessary to start the project</t>
+  </si>
+  <si>
+    <t>Clarify which components are available at Tec</t>
+  </si>
+  <si>
+    <t>Perform PO for missing components</t>
+  </si>
+  <si>
+    <t>Electronic Components</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Funding</t>
+  </si>
+  <si>
+    <t>Horizon 2020</t>
+  </si>
+  <si>
+    <t>Funding Programs: EU</t>
+  </si>
+  <si>
+    <t>Funding Programs: Mexico</t>
+  </si>
+  <si>
+    <t>Funding Programs: Jalisco</t>
+  </si>
+  <si>
+    <t>Funding Programs: Germany</t>
+  </si>
+  <si>
+    <t>Crowdfunding</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>Tax Consulting</t>
+  </si>
+  <si>
+    <t>Accounting Tool</t>
+  </si>
+  <si>
+    <t>HR Tool</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Analyze main competitors</t>
+  </si>
+  <si>
+    <t>Estimate financial situation for the company's first 5 years</t>
+  </si>
+  <si>
+    <t>Financial Analysis</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Define plan for marketing campaign for product's kick-off</t>
+  </si>
+  <si>
+    <t>Evaluate impact of Hackathon wih prototype</t>
+  </si>
+  <si>
+    <t>Investigate requirements for UG and GmbH foundation</t>
+  </si>
+  <si>
+    <t>Investigate requirements for S.A. de C.V. foundation</t>
+  </si>
+  <si>
+    <t>Found UG or GmbH</t>
+  </si>
+  <si>
+    <t>Investigate collaboration or synergy between S.A. de C.V. and UG/GmbH</t>
+  </si>
+  <si>
+    <t>Found S.A. de C.V. (if needed)</t>
+  </si>
+  <si>
+    <t>Receive 3 RFQs from tax consultants in Germany</t>
+  </si>
+  <si>
+    <t>Receive 3 RFQs from tax consultants in Mexico (if needed)</t>
+  </si>
+  <si>
+    <t>Hire tax consultant in Mexico (if needed)</t>
+  </si>
+  <si>
+    <t>Hire tax consultant in Germany</t>
+  </si>
+  <si>
+    <t>Investigate accounting tools</t>
+  </si>
+  <si>
+    <t>Define accounting tool to be used</t>
+  </si>
+  <si>
+    <t>Define tool to be used for company's email (e.g., tool to conect external email to email account)</t>
+  </si>
+  <si>
+    <t>Generate initial emails with company's website</t>
+  </si>
+  <si>
+    <t>Receive 3 RFQs to outsource website</t>
+  </si>
+  <si>
+    <t>Outsource website design (Front End)</t>
+  </si>
+  <si>
+    <t>Integrate Web Solution to company's website (Front End)</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Import/Export</t>
+  </si>
+  <si>
+    <t>Make feasibility analysis ofr crowdfunding campaign</t>
+  </si>
+  <si>
+    <t>Company Profile</t>
+  </si>
+  <si>
+    <t>Create company's description</t>
+  </si>
+  <si>
+    <t>Generate profile of company's members</t>
+  </si>
+  <si>
+    <t>Intellectual Property</t>
+  </si>
+  <si>
+    <t>International Patent</t>
+  </si>
+  <si>
+    <t>European Patent</t>
+  </si>
+  <si>
+    <t>US Patent</t>
+  </si>
+  <si>
+    <t>General Information</t>
   </si>
 </sst>
 </file>
@@ -945,70 +1171,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1293,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG58"/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1303,7 +1529,7 @@
     <col min="2" max="2" width="32.453125" style="9" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" style="35" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" style="38" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="4.26953125" style="9" customWidth="1"/>
     <col min="7" max="7" width="3.81640625" style="14" customWidth="1"/>
     <col min="8" max="10" width="3.81640625" style="15" customWidth="1"/>
@@ -1321,109 +1547,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="59" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="67">
+      <c r="G1" s="50">
         <v>2018</v>
       </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="69"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="52"/>
     </row>
     <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="61"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64"/>
       <c r="F2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="64" t="s">
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="66" t="s">
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="64" t="s">
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="64" t="s">
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="64" t="s">
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="48"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
-      <c r="AF2" s="64"/>
-      <c r="AG2" s="65"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="48"/>
+      <c r="AG2" s="49"/>
     </row>
     <row r="3" spans="1:33" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="53"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="62"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="28" t="s">
         <v>3</v>
       </c>
@@ -1510,16 +1736,11 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A4" s="30">
-        <v>1</v>
-      </c>
+      <c r="A4" s="30"/>
       <c r="B4" s="7"/>
       <c r="C4" s="33"/>
       <c r="D4" s="36"/>
-      <c r="E4" s="39">
-        <f>D4-C4</f>
-        <v>0</v>
-      </c>
+      <c r="E4" s="39"/>
       <c r="F4" s="7"/>
       <c r="G4" s="10"/>
       <c r="H4" s="4"/>
@@ -3441,6 +3662,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="AC2:AG2"/>
     <mergeCell ref="G1:AG1"/>
     <mergeCell ref="G2:K2"/>
@@ -3448,11 +3674,6 @@
     <mergeCell ref="P2:T2"/>
     <mergeCell ref="U2:X2"/>
     <mergeCell ref="Y2:AB2"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3461,435 +3682,721 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.7265625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="39.90625" style="43" customWidth="1"/>
+    <col min="3" max="5" width="41.90625" style="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B27" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B31" s="43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B33" s="43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B41" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B42" s="43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B43" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B44" s="43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.90625" style="43" customWidth="1"/>
-    <col min="2" max="4" width="41.90625" style="46" customWidth="1"/>
+    <col min="1" max="5" width="34.36328125" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
-        <v>14</v>
+        <v>171</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="45" t="s">
+        <v>174</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
-        <v>16</v>
+        <v>172</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>175</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
-        <v>17</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>176</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
-        <v>42</v>
+        <v>156</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="45" t="s">
+        <v>127</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="43" t="s">
-        <v>30</v>
+        <v>158</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>129</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
-        <v>33</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="46" t="s">
+        <v>130</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="43" t="s">
-        <v>29</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
+        <v>131</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="43" t="s">
-        <v>31</v>
+        <v>145</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="46" t="s">
+        <v>149</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="43" t="s">
-        <v>34</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="45" t="s">
+        <v>151</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
-        <v>19</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
+        <v>150</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="44" t="s">
-        <v>20</v>
+        <v>161</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="45" t="s">
+        <v>152</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="43" t="s">
-        <v>36</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="46" t="s">
+        <v>154</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="43" t="s">
-        <v>24</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="45" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B17" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="42" t="s">
-        <v>25</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="43" t="s">
-        <v>26</v>
-      </c>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="43" t="s">
-        <v>28</v>
-      </c>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="42" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="43" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="43" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="43" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="43" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="42" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="43" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="43" t="s">
-        <v>48</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update after meeting 28.08.
Update after meeting 28.08.
</commit_message>
<xml_diff>
--- a/Project_Management.xlsx
+++ b/Project_Management.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uidr0059\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6DB1F609-E721-449E-9B92-34FBE60A6254}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Phase 1'!$A$1:$F$3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Lopez Arce Vivas, Eduardo</author>
   </authors>
   <commentList>
-    <comment ref="B88" authorId="0" shapeId="0">
+    <comment ref="B88" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B92" authorId="0" shapeId="0">
+    <comment ref="B92" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B98" authorId="0" shapeId="0">
+    <comment ref="B98" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B99" authorId="0" shapeId="0">
+    <comment ref="B99" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B101" authorId="0" shapeId="0">
+    <comment ref="B101" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B109" authorId="0" shapeId="0">
+    <comment ref="B109" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -173,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B113" authorId="0" shapeId="0">
+    <comment ref="B113" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -197,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B117" authorId="0" shapeId="0">
+    <comment ref="B117" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -222,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B133" authorId="0" shapeId="0">
+    <comment ref="B133" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -247,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B139" authorId="0" shapeId="0">
+    <comment ref="B139" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -1427,7 +1428,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -3154,6 +3155,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3206,39 +3240,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3497,14 +3498,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>142870</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76195</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>119060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>142870</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76195</xdr:colOff>
       <xdr:row>217</xdr:row>
       <xdr:rowOff>138110</xdr:rowOff>
     </xdr:to>
@@ -3521,8 +3522,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9620245" y="559591"/>
-          <a:ext cx="0" cy="41381363"/>
+          <a:off x="10344145" y="547685"/>
+          <a:ext cx="0" cy="39385875"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3815,14 +3816,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW956"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C130" sqref="C130"/>
+      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3855,58 +3856,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="292" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="278" t="s">
+      <c r="B1" s="289" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="293" t="s">
+      <c r="C1" s="304" t="s">
         <v>371</v>
       </c>
-      <c r="D1" s="284" t="s">
+      <c r="D1" s="295" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="287" t="s">
+      <c r="E1" s="298" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="290" t="s">
+      <c r="F1" s="301" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="298">
+      <c r="H1" s="280">
         <v>2018</v>
       </c>
-      <c r="I1" s="299"/>
-      <c r="J1" s="299"/>
-      <c r="K1" s="299"/>
-      <c r="L1" s="299"/>
-      <c r="M1" s="299"/>
-      <c r="N1" s="299"/>
-      <c r="O1" s="299"/>
-      <c r="P1" s="299"/>
-      <c r="Q1" s="299"/>
-      <c r="R1" s="299"/>
-      <c r="S1" s="299"/>
-      <c r="T1" s="299"/>
-      <c r="U1" s="299"/>
-      <c r="V1" s="299"/>
-      <c r="W1" s="299"/>
-      <c r="X1" s="299"/>
-      <c r="Y1" s="299"/>
-      <c r="Z1" s="299"/>
-      <c r="AA1" s="299"/>
-      <c r="AB1" s="299"/>
-      <c r="AC1" s="299"/>
-      <c r="AD1" s="299"/>
-      <c r="AE1" s="299"/>
-      <c r="AF1" s="299"/>
-      <c r="AG1" s="299"/>
-      <c r="AH1" s="299"/>
-      <c r="AI1" s="299"/>
-      <c r="AJ1" s="300"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
+      <c r="N1" s="281"/>
+      <c r="O1" s="281"/>
+      <c r="P1" s="281"/>
+      <c r="Q1" s="281"/>
+      <c r="R1" s="281"/>
+      <c r="S1" s="281"/>
+      <c r="T1" s="281"/>
+      <c r="U1" s="281"/>
+      <c r="V1" s="281"/>
+      <c r="W1" s="281"/>
+      <c r="X1" s="281"/>
+      <c r="Y1" s="281"/>
+      <c r="Z1" s="281"/>
+      <c r="AA1" s="281"/>
+      <c r="AB1" s="281"/>
+      <c r="AC1" s="281"/>
+      <c r="AD1" s="281"/>
+      <c r="AE1" s="281"/>
+      <c r="AF1" s="281"/>
+      <c r="AG1" s="281"/>
+      <c r="AH1" s="281"/>
+      <c r="AI1" s="281"/>
+      <c r="AJ1" s="282"/>
       <c r="AK1" s="205" t="s">
         <v>374</v>
       </c>
@@ -3920,77 +3921,77 @@
       </c>
     </row>
     <row r="2" spans="1:49" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="282"/>
-      <c r="B2" s="279"/>
-      <c r="C2" s="294"/>
-      <c r="D2" s="285"/>
-      <c r="E2" s="288"/>
-      <c r="F2" s="291"/>
+      <c r="A2" s="293"/>
+      <c r="B2" s="290"/>
+      <c r="C2" s="305"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="299"/>
+      <c r="F2" s="302"/>
       <c r="G2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="296" t="s">
+      <c r="H2" s="278" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="297"/>
-      <c r="J2" s="303" t="s">
+      <c r="I2" s="279"/>
+      <c r="J2" s="285" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="301"/>
-      <c r="L2" s="301"/>
-      <c r="M2" s="301"/>
-      <c r="N2" s="302"/>
-      <c r="O2" s="301" t="s">
+      <c r="K2" s="283"/>
+      <c r="L2" s="283"/>
+      <c r="M2" s="283"/>
+      <c r="N2" s="284"/>
+      <c r="O2" s="283" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="301"/>
-      <c r="Q2" s="301"/>
-      <c r="R2" s="301"/>
-      <c r="S2" s="304" t="s">
+      <c r="P2" s="283"/>
+      <c r="Q2" s="283"/>
+      <c r="R2" s="283"/>
+      <c r="S2" s="286" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="305"/>
-      <c r="U2" s="305"/>
-      <c r="V2" s="303"/>
-      <c r="W2" s="306" t="s">
+      <c r="T2" s="287"/>
+      <c r="U2" s="287"/>
+      <c r="V2" s="285"/>
+      <c r="W2" s="288" t="s">
         <v>7</v>
       </c>
-      <c r="X2" s="301"/>
-      <c r="Y2" s="301"/>
-      <c r="Z2" s="301"/>
-      <c r="AA2" s="302"/>
-      <c r="AB2" s="301" t="s">
+      <c r="X2" s="283"/>
+      <c r="Y2" s="283"/>
+      <c r="Z2" s="283"/>
+      <c r="AA2" s="284"/>
+      <c r="AB2" s="283" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="301"/>
-      <c r="AD2" s="301"/>
-      <c r="AE2" s="302"/>
-      <c r="AF2" s="301" t="s">
+      <c r="AC2" s="283"/>
+      <c r="AD2" s="283"/>
+      <c r="AE2" s="284"/>
+      <c r="AF2" s="283" t="s">
         <v>9</v>
       </c>
-      <c r="AG2" s="301"/>
-      <c r="AH2" s="301"/>
-      <c r="AI2" s="301"/>
-      <c r="AJ2" s="302"/>
+      <c r="AG2" s="283"/>
+      <c r="AH2" s="283"/>
+      <c r="AI2" s="283"/>
+      <c r="AJ2" s="284"/>
       <c r="AK2" s="205" t="s">
         <v>373</v>
       </c>
       <c r="AL2" s="209">
         <f>COUNTIFS(C:C,"Doing")</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AM2" s="207">
         <f>AL2/(AL3+AL2+AL1)</f>
-        <v>0.18248175182481752</v>
+        <v>0.16058394160583941</v>
       </c>
     </row>
     <row r="3" spans="1:49" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="283"/>
-      <c r="B3" s="280"/>
-      <c r="C3" s="295"/>
-      <c r="D3" s="286"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="292"/>
+      <c r="A3" s="294"/>
+      <c r="B3" s="291"/>
+      <c r="C3" s="306"/>
+      <c r="D3" s="297"/>
+      <c r="E3" s="300"/>
+      <c r="F3" s="303"/>
       <c r="G3" s="47" t="s">
         <v>3</v>
       </c>
@@ -4086,11 +4087,11 @@
       </c>
       <c r="AL3" s="210">
         <f>COUNTIFS(C:C,"Closed")</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AM3" s="207">
         <f>AL3/(AL3+AL2+AL1)</f>
-        <v>0.11678832116788321</v>
+        <v>0.13868613138686131</v>
       </c>
     </row>
     <row r="4" spans="1:49" s="78" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4306,7 +4307,7 @@
         <v>103</v>
       </c>
       <c r="C8" s="225" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D8" s="112">
         <v>43275</v>
@@ -4577,7 +4578,7 @@
         <v>189</v>
       </c>
       <c r="C14" s="232" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D14" s="38">
         <v>43311</v>
@@ -4621,7 +4622,7 @@
         <v>104</v>
       </c>
       <c r="C15" s="236" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D15" s="110">
         <v>43275</v>
@@ -36127,8 +36128,14 @@
       <c r="AJ956" s="230"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F3"/>
+  <autoFilter ref="A1:F3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="14">
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="C1:C3"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H1:AJ1"/>
     <mergeCell ref="AF2:AJ2"/>
@@ -36137,12 +36144,6 @@
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="S2:V2"/>
     <mergeCell ref="W2:AA2"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="C1:C3"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Closed">
@@ -36153,7 +36154,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Open,Doing,Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -36169,7 +36170,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36677,7 +36678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>